<commit_message>
complete overhaul, with roster object per file, new and cleaned structure of shifts and cleaned print statements
</commit_message>
<xml_diff>
--- a/jeremy-project/sheet2.xlsx
+++ b/jeremy-project/sheet2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="78">
   <si>
     <r>
       <t>Centre Assistant Roster - Week One -</t>
@@ -313,10 +313,7 @@
     </r>
   </si>
   <si>
-    <t>11am-6.30pm</t>
-  </si>
-  <si>
-    <t>11am - 6.30pm</t>
+    <t>11am - 3pm/4pm-7.30pm</t>
   </si>
 </sst>
 </file>
@@ -961,6 +958,51 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -987,51 +1029,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1337,28 +1334,27 @@
   <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="16.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="71"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1438,7 +1434,7 @@
       <c r="H4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="57">
+      <c r="I4" s="48">
         <v>17</v>
       </c>
     </row>
@@ -1461,7 +1457,7 @@
       <c r="H5" s="16">
         <v>4</v>
       </c>
-      <c r="I5" s="58"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" ht="16">
       <c r="A6" s="21" t="s">
@@ -1474,7 +1470,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="18"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="57">
+      <c r="I6" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1489,7 +1485,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="58"/>
+      <c r="I7" s="49"/>
     </row>
     <row r="8" spans="1:9" ht="16">
       <c r="A8" s="21" t="s">
@@ -1499,7 +1495,7 @@
         <v>77</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="10" t="s">
@@ -1512,7 +1508,7 @@
       <c r="H8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="48">
         <v>27.5</v>
       </c>
     </row>
@@ -1537,7 +1533,7 @@
       <c r="H9" s="16">
         <v>6.5</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:9" ht="16">
       <c r="A10" s="21" t="s">
@@ -1562,7 +1558,7 @@
       <c r="H10" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="57">
+      <c r="I10" s="48">
         <v>31</v>
       </c>
     </row>
@@ -1589,7 +1585,7 @@
       <c r="H11" s="16">
         <v>6.5</v>
       </c>
-      <c r="I11" s="58"/>
+      <c r="I11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16">
       <c r="A12" s="21" t="s">
@@ -1602,7 +1598,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="57">
+      <c r="I12" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1617,7 +1613,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="58"/>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:9" ht="16">
       <c r="A14" s="21" t="s">
@@ -1636,7 +1632,7 @@
       <c r="H14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="48">
         <v>16.5</v>
       </c>
     </row>
@@ -1657,22 +1653,22 @@
       <c r="H15" s="16">
         <v>5</v>
       </c>
-      <c r="I15" s="58"/>
+      <c r="I15" s="49"/>
     </row>
     <row r="16" spans="1:9" ht="66.75" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
     </row>
     <row r="17" spans="1:9" ht="16">
       <c r="A17" s="21" t="s">
@@ -1685,7 +1681,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="57">
+      <c r="I17" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1700,7 +1696,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="58"/>
+      <c r="I18" s="49"/>
     </row>
     <row r="19" spans="1:9" ht="16">
       <c r="A19" s="21" t="s">
@@ -1713,7 +1709,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="57">
+      <c r="I19" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1728,7 +1724,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="58"/>
+      <c r="I20" s="49"/>
     </row>
     <row r="21" spans="1:9" ht="16">
       <c r="A21" s="21" t="s">
@@ -1741,7 +1737,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="57">
+      <c r="I21" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1756,7 +1752,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="15"/>
       <c r="H22" s="26"/>
-      <c r="I22" s="58"/>
+      <c r="I22" s="49"/>
     </row>
     <row r="23" spans="1:9" ht="16">
       <c r="A23" s="21" t="s">
@@ -1771,7 +1767,7 @@
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="57">
+      <c r="I23" s="48">
         <v>4</v>
       </c>
     </row>
@@ -1788,7 +1784,7 @@
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="58"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:9" ht="16">
       <c r="A25" s="21" t="s">
@@ -1809,7 +1805,7 @@
         <v>22</v>
       </c>
       <c r="H25" s="10"/>
-      <c r="I25" s="57">
+      <c r="I25" s="48">
         <v>26</v>
       </c>
     </row>
@@ -1832,7 +1828,7 @@
         <v>6.5</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="58"/>
+      <c r="I26" s="49"/>
     </row>
     <row r="27" spans="1:9" ht="16">
       <c r="A27" s="21" t="s">
@@ -1857,7 +1853,7 @@
       <c r="H27" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="57">
+      <c r="I27" s="48">
         <v>19</v>
       </c>
     </row>
@@ -1884,22 +1880,22 @@
       <c r="H28" s="15">
         <v>3</v>
       </c>
-      <c r="I28" s="58"/>
+      <c r="I28" s="49"/>
     </row>
     <row r="29" spans="1:9" ht="16">
       <c r="A29" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57">
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1914,7 +1910,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="58"/>
+      <c r="I30" s="49"/>
     </row>
     <row r="31" spans="1:9" ht="16">
       <c r="A31" s="21" t="s">
@@ -1927,7 +1923,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
-      <c r="I31" s="57">
+      <c r="I31" s="48">
         <v>0</v>
       </c>
     </row>
@@ -1942,7 +1938,7 @@
       <c r="F32" s="14"/>
       <c r="G32" s="15"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="58"/>
+      <c r="I32" s="49"/>
     </row>
     <row r="33" spans="1:9" ht="16">
       <c r="A33" s="21" t="s">
@@ -1963,7 +1959,7 @@
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="57">
+      <c r="I33" s="48">
         <v>12</v>
       </c>
     </row>
@@ -1986,7 +1982,7 @@
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="58"/>
+      <c r="I34" s="49"/>
     </row>
     <row r="35" spans="1:9" ht="16">
       <c r="A35" s="21" t="s">
@@ -2005,7 +2001,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="11"/>
-      <c r="I35" s="57">
+      <c r="I35" s="48">
         <v>10</v>
       </c>
     </row>
@@ -2026,7 +2022,7 @@
         <v>4</v>
       </c>
       <c r="H36" s="16"/>
-      <c r="I36" s="58"/>
+      <c r="I36" s="49"/>
     </row>
     <row r="37" spans="1:9" ht="16">
       <c r="A37" s="21" t="s">
@@ -2039,7 +2035,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="57">
+      <c r="I37" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2054,7 +2050,7 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="58"/>
+      <c r="I38" s="49"/>
     </row>
     <row r="39" spans="1:9" ht="16">
       <c r="A39" s="21" t="s">
@@ -2073,7 +2069,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="19"/>
-      <c r="I39" s="57">
+      <c r="I39" s="48">
         <v>12</v>
       </c>
     </row>
@@ -2094,7 +2090,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="15"/>
       <c r="H40" s="14"/>
-      <c r="I40" s="58"/>
+      <c r="I40" s="49"/>
     </row>
     <row r="41" spans="1:9" ht="16">
       <c r="A41" s="21" t="s">
@@ -2113,7 +2109,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
-      <c r="I41" s="57">
+      <c r="I41" s="48">
         <v>17</v>
       </c>
     </row>
@@ -2134,7 +2130,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="15"/>
       <c r="H42" s="14"/>
-      <c r="I42" s="58"/>
+      <c r="I42" s="49"/>
     </row>
     <row r="43" spans="1:9" ht="16">
       <c r="A43" s="21" t="s">
@@ -2147,7 +2143,7 @@
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="20"/>
-      <c r="I43" s="57">
+      <c r="I43" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2162,7 +2158,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="15"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="58"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="1:9" ht="16">
       <c r="A45" s="29" t="s">
@@ -2194,13 +2190,13 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16">
-      <c r="A46" s="62" t="s">
+      <c r="A46" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="62"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2281,7 +2277,7 @@
       <c r="H49" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I49" s="57">
+      <c r="I49" s="48">
         <v>17</v>
       </c>
     </row>
@@ -2304,7 +2300,7 @@
       <c r="H50" s="16">
         <v>5</v>
       </c>
-      <c r="I50" s="58"/>
+      <c r="I50" s="49"/>
     </row>
     <row r="51" spans="1:9" ht="16">
       <c r="A51" s="21" t="s">
@@ -2317,7 +2313,7 @@
       <c r="F51" s="19"/>
       <c r="G51" s="18"/>
       <c r="H51" s="20"/>
-      <c r="I51" s="57">
+      <c r="I51" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2332,7 +2328,7 @@
       <c r="F52" s="14"/>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="58"/>
+      <c r="I52" s="49"/>
     </row>
     <row r="53" spans="1:9" ht="16">
       <c r="A53" s="21" t="s">
@@ -2355,7 +2351,7 @@
       <c r="H53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="57">
+      <c r="I53" s="48">
         <v>23.5</v>
       </c>
     </row>
@@ -2380,7 +2376,7 @@
       <c r="H54" s="16">
         <v>5</v>
       </c>
-      <c r="I54" s="58"/>
+      <c r="I54" s="49"/>
     </row>
     <row r="55" spans="1:9" ht="16">
       <c r="A55" s="21" t="s">
@@ -2403,7 +2399,7 @@
       <c r="H55" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="57">
+      <c r="I55" s="48">
         <v>19</v>
       </c>
     </row>
@@ -2428,7 +2424,7 @@
       <c r="H56" s="16">
         <v>3</v>
       </c>
-      <c r="I56" s="58"/>
+      <c r="I56" s="49"/>
     </row>
     <row r="57" spans="1:9" ht="16">
       <c r="A57" s="21" t="s">
@@ -2445,7 +2441,7 @@
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="H57" s="20"/>
-      <c r="I57" s="57">
+      <c r="I57" s="48">
         <v>9</v>
       </c>
     </row>
@@ -2464,7 +2460,7 @@
       <c r="F58" s="14"/>
       <c r="G58" s="15"/>
       <c r="H58" s="16"/>
-      <c r="I58" s="58"/>
+      <c r="I58" s="49"/>
     </row>
     <row r="59" spans="1:9" ht="16">
       <c r="A59" s="21" t="s">
@@ -2487,7 +2483,7 @@
       <c r="H59" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I59" s="57">
+      <c r="I59" s="48">
         <v>24.5</v>
       </c>
     </row>
@@ -2512,20 +2508,20 @@
       <c r="H60" s="14">
         <v>4</v>
       </c>
-      <c r="I60" s="58"/>
+      <c r="I60" s="49"/>
     </row>
     <row r="61" spans="1:9" ht="16">
       <c r="A61" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="63"/>
-      <c r="C61" s="64"/>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="65"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="62"/>
     </row>
     <row r="62" spans="1:9" ht="16">
       <c r="A62" s="21" t="s">
@@ -2538,7 +2534,7 @@
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
       <c r="H62" s="20"/>
-      <c r="I62" s="57">
+      <c r="I62" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2553,7 +2549,7 @@
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
       <c r="H63" s="16"/>
-      <c r="I63" s="58"/>
+      <c r="I63" s="49"/>
     </row>
     <row r="64" spans="1:9" ht="16">
       <c r="A64" s="21" t="s">
@@ -2570,7 +2566,7 @@
         <v>15</v>
       </c>
       <c r="H64" s="11"/>
-      <c r="I64" s="57">
+      <c r="I64" s="48">
         <v>7</v>
       </c>
     </row>
@@ -2589,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="H65" s="16"/>
-      <c r="I65" s="58"/>
+      <c r="I65" s="49"/>
     </row>
     <row r="66" spans="1:9" ht="16">
       <c r="A66" s="21" t="s">
@@ -2602,7 +2598,7 @@
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="25"/>
-      <c r="I66" s="57">
+      <c r="I66" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2617,7 +2613,7 @@
       <c r="F67" s="14"/>
       <c r="G67" s="15"/>
       <c r="H67" s="26"/>
-      <c r="I67" s="58"/>
+      <c r="I67" s="49"/>
     </row>
     <row r="68" spans="1:9" ht="16">
       <c r="A68" s="21" t="s">
@@ -2634,7 +2630,7 @@
       <c r="F68" s="27"/>
       <c r="G68" s="10"/>
       <c r="H68" s="11"/>
-      <c r="I68" s="57">
+      <c r="I68" s="48">
         <v>8</v>
       </c>
     </row>
@@ -2653,7 +2649,7 @@
       <c r="F69" s="14"/>
       <c r="G69" s="15"/>
       <c r="H69" s="16"/>
-      <c r="I69" s="58"/>
+      <c r="I69" s="49"/>
     </row>
     <row r="70" spans="1:9" ht="16">
       <c r="A70" s="21" t="s">
@@ -2676,7 +2672,7 @@
         <v>13</v>
       </c>
       <c r="H70" s="10"/>
-      <c r="I70" s="57">
+      <c r="I70" s="48">
         <v>19.5</v>
       </c>
     </row>
@@ -2701,7 +2697,7 @@
         <v>3</v>
       </c>
       <c r="H71" s="14"/>
-      <c r="I71" s="58"/>
+      <c r="I71" s="49"/>
     </row>
     <row r="72" spans="1:9" ht="16">
       <c r="A72" s="21" t="s">
@@ -2722,7 +2718,7 @@
         <v>14</v>
       </c>
       <c r="H72" s="11"/>
-      <c r="I72" s="57">
+      <c r="I72" s="48">
         <v>17</v>
       </c>
     </row>
@@ -2745,22 +2741,22 @@
         <v>5</v>
       </c>
       <c r="H73" s="16"/>
-      <c r="I73" s="58"/>
+      <c r="I73" s="49"/>
     </row>
     <row r="74" spans="1:9" ht="16">
       <c r="A74" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B74" s="59" t="s">
+      <c r="B74" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="60"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="60"/>
-      <c r="G74" s="60"/>
-      <c r="H74" s="61"/>
-      <c r="I74" s="57">
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2775,7 +2771,7 @@
       <c r="F75" s="14"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15"/>
-      <c r="I75" s="58"/>
+      <c r="I75" s="49"/>
     </row>
     <row r="76" spans="1:9" ht="16">
       <c r="A76" s="21" t="s">
@@ -2788,7 +2784,7 @@
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
       <c r="H76" s="11"/>
-      <c r="I76" s="57">
+      <c r="I76" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2803,7 +2799,7 @@
       <c r="F77" s="14"/>
       <c r="G77" s="15"/>
       <c r="H77" s="16"/>
-      <c r="I77" s="58"/>
+      <c r="I77" s="49"/>
     </row>
     <row r="78" spans="1:9" ht="16">
       <c r="A78" s="21" t="s">
@@ -2816,7 +2812,7 @@
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
       <c r="H78" s="20"/>
-      <c r="I78" s="57">
+      <c r="I78" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2831,7 +2827,7 @@
       <c r="F79" s="14"/>
       <c r="G79" s="15"/>
       <c r="H79" s="16"/>
-      <c r="I79" s="58"/>
+      <c r="I79" s="49"/>
     </row>
     <row r="80" spans="1:9" ht="16">
       <c r="A80" s="21" t="s">
@@ -2850,7 +2846,7 @@
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="11"/>
-      <c r="I80" s="57">
+      <c r="I80" s="48">
         <v>14.5</v>
       </c>
     </row>
@@ -2871,7 +2867,7 @@
       <c r="F81" s="14"/>
       <c r="G81" s="15"/>
       <c r="H81" s="16"/>
-      <c r="I81" s="58"/>
+      <c r="I81" s="49"/>
     </row>
     <row r="82" spans="1:9" ht="16">
       <c r="A82" s="21" t="s">
@@ -2884,7 +2880,7 @@
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
-      <c r="I82" s="57">
+      <c r="I82" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2899,7 +2895,7 @@
       <c r="F83" s="14"/>
       <c r="G83" s="15"/>
       <c r="H83" s="15"/>
-      <c r="I83" s="58"/>
+      <c r="I83" s="49"/>
     </row>
     <row r="84" spans="1:9" ht="16">
       <c r="A84" s="21" t="s">
@@ -2912,7 +2908,7 @@
       <c r="F84" s="19"/>
       <c r="G84" s="19"/>
       <c r="H84" s="19"/>
-      <c r="I84" s="57">
+      <c r="I84" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2927,7 +2923,7 @@
       <c r="F85" s="14"/>
       <c r="G85" s="15"/>
       <c r="H85" s="14"/>
-      <c r="I85" s="58"/>
+      <c r="I85" s="49"/>
     </row>
     <row r="86" spans="1:9" ht="16">
       <c r="A86" s="21" t="s">
@@ -2950,7 +2946,7 @@
       <c r="H86" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I86" s="57">
+      <c r="I86" s="48">
         <v>21.5</v>
       </c>
     </row>
@@ -2975,7 +2971,7 @@
       <c r="H87" s="14">
         <v>6.5</v>
       </c>
-      <c r="I87" s="58"/>
+      <c r="I87" s="49"/>
     </row>
     <row r="88" spans="1:9" ht="16">
       <c r="A88" s="21" t="s">
@@ -2988,7 +2984,7 @@
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
       <c r="H88" s="20"/>
-      <c r="I88" s="57">
+      <c r="I88" s="48">
         <v>0</v>
       </c>
     </row>
@@ -3003,7 +2999,7 @@
       <c r="F89" s="14"/>
       <c r="G89" s="15"/>
       <c r="H89" s="16"/>
-      <c r="I89" s="58"/>
+      <c r="I89" s="49"/>
     </row>
     <row r="90" spans="1:9" ht="17" thickBot="1">
       <c r="A90" s="29" t="s">
@@ -3035,149 +3031,149 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" thickTop="1">
-      <c r="A91" s="48" t="s">
+      <c r="A91" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="50"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
+      <c r="I91" s="65"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="51"/>
-      <c r="B92" s="52"/>
-      <c r="C92" s="52"/>
-      <c r="D92" s="52"/>
-      <c r="E92" s="52"/>
-      <c r="F92" s="52"/>
-      <c r="G92" s="52"/>
-      <c r="H92" s="52"/>
-      <c r="I92" s="53"/>
+      <c r="A92" s="66"/>
+      <c r="B92" s="67"/>
+      <c r="C92" s="67"/>
+      <c r="D92" s="67"/>
+      <c r="E92" s="67"/>
+      <c r="F92" s="67"/>
+      <c r="G92" s="67"/>
+      <c r="H92" s="67"/>
+      <c r="I92" s="68"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="51"/>
-      <c r="B93" s="52"/>
-      <c r="C93" s="52"/>
-      <c r="D93" s="52"/>
-      <c r="E93" s="52"/>
-      <c r="F93" s="52"/>
-      <c r="G93" s="52"/>
-      <c r="H93" s="52"/>
-      <c r="I93" s="53"/>
+      <c r="A93" s="66"/>
+      <c r="B93" s="67"/>
+      <c r="C93" s="67"/>
+      <c r="D93" s="67"/>
+      <c r="E93" s="67"/>
+      <c r="F93" s="67"/>
+      <c r="G93" s="67"/>
+      <c r="H93" s="67"/>
+      <c r="I93" s="68"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="51"/>
-      <c r="B94" s="52"/>
-      <c r="C94" s="52"/>
-      <c r="D94" s="52"/>
-      <c r="E94" s="52"/>
-      <c r="F94" s="52"/>
-      <c r="G94" s="52"/>
-      <c r="H94" s="52"/>
-      <c r="I94" s="53"/>
+      <c r="A94" s="66"/>
+      <c r="B94" s="67"/>
+      <c r="C94" s="67"/>
+      <c r="D94" s="67"/>
+      <c r="E94" s="67"/>
+      <c r="F94" s="67"/>
+      <c r="G94" s="67"/>
+      <c r="H94" s="67"/>
+      <c r="I94" s="68"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="51"/>
-      <c r="B95" s="52"/>
-      <c r="C95" s="52"/>
-      <c r="D95" s="52"/>
-      <c r="E95" s="52"/>
-      <c r="F95" s="52"/>
-      <c r="G95" s="52"/>
-      <c r="H95" s="52"/>
-      <c r="I95" s="53"/>
+      <c r="A95" s="66"/>
+      <c r="B95" s="67"/>
+      <c r="C95" s="67"/>
+      <c r="D95" s="67"/>
+      <c r="E95" s="67"/>
+      <c r="F95" s="67"/>
+      <c r="G95" s="67"/>
+      <c r="H95" s="67"/>
+      <c r="I95" s="68"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="51"/>
-      <c r="B96" s="52"/>
-      <c r="C96" s="52"/>
-      <c r="D96" s="52"/>
-      <c r="E96" s="52"/>
-      <c r="F96" s="52"/>
-      <c r="G96" s="52"/>
-      <c r="H96" s="52"/>
-      <c r="I96" s="53"/>
+      <c r="A96" s="66"/>
+      <c r="B96" s="67"/>
+      <c r="C96" s="67"/>
+      <c r="D96" s="67"/>
+      <c r="E96" s="67"/>
+      <c r="F96" s="67"/>
+      <c r="G96" s="67"/>
+      <c r="H96" s="67"/>
+      <c r="I96" s="68"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="51"/>
-      <c r="B97" s="52"/>
-      <c r="C97" s="52"/>
-      <c r="D97" s="52"/>
-      <c r="E97" s="52"/>
-      <c r="F97" s="52"/>
-      <c r="G97" s="52"/>
-      <c r="H97" s="52"/>
-      <c r="I97" s="53"/>
+      <c r="A97" s="66"/>
+      <c r="B97" s="67"/>
+      <c r="C97" s="67"/>
+      <c r="D97" s="67"/>
+      <c r="E97" s="67"/>
+      <c r="F97" s="67"/>
+      <c r="G97" s="67"/>
+      <c r="H97" s="67"/>
+      <c r="I97" s="68"/>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="51"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
-      <c r="E98" s="52"/>
-      <c r="F98" s="52"/>
-      <c r="G98" s="52"/>
-      <c r="H98" s="52"/>
-      <c r="I98" s="53"/>
+      <c r="A98" s="66"/>
+      <c r="B98" s="67"/>
+      <c r="C98" s="67"/>
+      <c r="D98" s="67"/>
+      <c r="E98" s="67"/>
+      <c r="F98" s="67"/>
+      <c r="G98" s="67"/>
+      <c r="H98" s="67"/>
+      <c r="I98" s="68"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="51"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="52"/>
-      <c r="D99" s="52"/>
-      <c r="E99" s="52"/>
-      <c r="F99" s="52"/>
-      <c r="G99" s="52"/>
-      <c r="H99" s="52"/>
-      <c r="I99" s="53"/>
+      <c r="A99" s="66"/>
+      <c r="B99" s="67"/>
+      <c r="C99" s="67"/>
+      <c r="D99" s="67"/>
+      <c r="E99" s="67"/>
+      <c r="F99" s="67"/>
+      <c r="G99" s="67"/>
+      <c r="H99" s="67"/>
+      <c r="I99" s="68"/>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="51"/>
-      <c r="B100" s="52"/>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
-      <c r="E100" s="52"/>
-      <c r="F100" s="52"/>
-      <c r="G100" s="52"/>
-      <c r="H100" s="52"/>
-      <c r="I100" s="53"/>
+      <c r="A100" s="66"/>
+      <c r="B100" s="67"/>
+      <c r="C100" s="67"/>
+      <c r="D100" s="67"/>
+      <c r="E100" s="67"/>
+      <c r="F100" s="67"/>
+      <c r="G100" s="67"/>
+      <c r="H100" s="67"/>
+      <c r="I100" s="68"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="51"/>
-      <c r="B101" s="52"/>
-      <c r="C101" s="52"/>
-      <c r="D101" s="52"/>
-      <c r="E101" s="52"/>
-      <c r="F101" s="52"/>
-      <c r="G101" s="52"/>
-      <c r="H101" s="52"/>
-      <c r="I101" s="53"/>
+      <c r="A101" s="66"/>
+      <c r="B101" s="67"/>
+      <c r="C101" s="67"/>
+      <c r="D101" s="67"/>
+      <c r="E101" s="67"/>
+      <c r="F101" s="67"/>
+      <c r="G101" s="67"/>
+      <c r="H101" s="67"/>
+      <c r="I101" s="68"/>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="51"/>
-      <c r="B102" s="52"/>
-      <c r="C102" s="52"/>
-      <c r="D102" s="52"/>
-      <c r="E102" s="52"/>
-      <c r="F102" s="52"/>
-      <c r="G102" s="52"/>
-      <c r="H102" s="52"/>
-      <c r="I102" s="53"/>
+      <c r="A102" s="66"/>
+      <c r="B102" s="67"/>
+      <c r="C102" s="67"/>
+      <c r="D102" s="67"/>
+      <c r="E102" s="67"/>
+      <c r="F102" s="67"/>
+      <c r="G102" s="67"/>
+      <c r="H102" s="67"/>
+      <c r="I102" s="68"/>
     </row>
     <row r="103" spans="1:9" ht="15" thickBot="1">
-      <c r="A103" s="54"/>
-      <c r="B103" s="55"/>
-      <c r="C103" s="55"/>
-      <c r="D103" s="55"/>
-      <c r="E103" s="55"/>
-      <c r="F103" s="55"/>
-      <c r="G103" s="55"/>
-      <c r="H103" s="55"/>
-      <c r="I103" s="56"/>
+      <c r="A103" s="69"/>
+      <c r="B103" s="70"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="70"/>
+      <c r="E103" s="70"/>
+      <c r="F103" s="70"/>
+      <c r="G103" s="70"/>
+      <c r="H103" s="70"/>
+      <c r="I103" s="71"/>
     </row>
     <row r="104" spans="1:9" ht="15" thickTop="1">
       <c r="A104" s="1"/>
@@ -3192,29 +3188,14 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="A91:I103"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I80:I81"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="B74:H74"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="I49:I50"/>
     <mergeCell ref="I78:I79"/>
@@ -3231,14 +3212,29 @@
     <mergeCell ref="I74:I75"/>
     <mergeCell ref="I76:I77"/>
     <mergeCell ref="I51:I52"/>
-    <mergeCell ref="A91:I103"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I80:I81"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I84:I85"/>
-    <mergeCell ref="I86:I87"/>
-    <mergeCell ref="I88:I89"/>
-    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
added the shiftDAL interface and did some house cleaning
</commit_message>
<xml_diff>
--- a/jeremy-project/sheet2.xlsx
+++ b/jeremy-project/sheet2.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="79">
   <si>
     <r>
       <t>Centre Assistant Roster - Week One -</t>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>11am - 3pm/4pm-7.30pm</t>
+  </si>
+  <si>
+    <t>11am - 3pm/4pm-7:45pm</t>
   </si>
 </sst>
 </file>
@@ -958,20 +961,59 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -982,53 +1024,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,7 +1337,7 @@
   <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1347,14 +1350,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1434,7 +1437,7 @@
       <c r="H4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="57">
         <v>17</v>
       </c>
     </row>
@@ -1457,7 +1460,7 @@
       <c r="H5" s="16">
         <v>4</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:9" ht="16">
       <c r="A6" s="21" t="s">
@@ -1470,7 +1473,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="18"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="48">
+      <c r="I6" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1485,14 +1488,14 @@
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="49"/>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:9" ht="16">
       <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>77</v>
@@ -1508,7 +1511,7 @@
       <c r="H8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="57">
         <v>27.5</v>
       </c>
     </row>
@@ -1533,7 +1536,7 @@
       <c r="H9" s="16">
         <v>6.5</v>
       </c>
-      <c r="I9" s="49"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" ht="16">
       <c r="A10" s="21" t="s">
@@ -1558,7 +1561,7 @@
       <c r="H10" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="57">
         <v>31</v>
       </c>
     </row>
@@ -1585,7 +1588,7 @@
       <c r="H11" s="16">
         <v>6.5</v>
       </c>
-      <c r="I11" s="49"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="16">
       <c r="A12" s="21" t="s">
@@ -1598,7 +1601,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="48">
+      <c r="I12" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1613,7 +1616,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" ht="16">
       <c r="A14" s="21" t="s">
@@ -1632,7 +1635,7 @@
       <c r="H14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="57">
         <v>16.5</v>
       </c>
     </row>
@@ -1653,22 +1656,22 @@
       <c r="H15" s="16">
         <v>5</v>
       </c>
-      <c r="I15" s="49"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9" ht="66.75" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="68"/>
     </row>
     <row r="17" spans="1:9" ht="16">
       <c r="A17" s="21" t="s">
@@ -1681,7 +1684,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="48">
+      <c r="I17" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1699,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="49"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" ht="16">
       <c r="A19" s="21" t="s">
@@ -1709,7 +1712,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="48">
+      <c r="I19" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1724,7 +1727,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="58"/>
     </row>
     <row r="21" spans="1:9" ht="16">
       <c r="A21" s="21" t="s">
@@ -1737,7 +1740,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="48">
+      <c r="I21" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1752,7 +1755,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="15"/>
       <c r="H22" s="26"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:9" ht="16">
       <c r="A23" s="21" t="s">
@@ -1767,7 +1770,7 @@
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="48">
+      <c r="I23" s="57">
         <v>4</v>
       </c>
     </row>
@@ -1784,7 +1787,7 @@
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="49"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9" ht="16">
       <c r="A25" s="21" t="s">
@@ -1805,7 +1808,7 @@
         <v>22</v>
       </c>
       <c r="H25" s="10"/>
-      <c r="I25" s="48">
+      <c r="I25" s="57">
         <v>26</v>
       </c>
     </row>
@@ -1828,7 +1831,7 @@
         <v>6.5</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="49"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:9" ht="16">
       <c r="A27" s="21" t="s">
@@ -1853,7 +1856,7 @@
       <c r="H27" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="48">
+      <c r="I27" s="57">
         <v>19</v>
       </c>
     </row>
@@ -1880,22 +1883,22 @@
       <c r="H28" s="15">
         <v>3</v>
       </c>
-      <c r="I28" s="49"/>
+      <c r="I28" s="58"/>
     </row>
     <row r="29" spans="1:9" ht="16">
       <c r="A29" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="48">
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1910,7 +1913,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="49"/>
+      <c r="I30" s="58"/>
     </row>
     <row r="31" spans="1:9" ht="16">
       <c r="A31" s="21" t="s">
@@ -1923,7 +1926,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
-      <c r="I31" s="48">
+      <c r="I31" s="57">
         <v>0</v>
       </c>
     </row>
@@ -1938,7 +1941,7 @@
       <c r="F32" s="14"/>
       <c r="G32" s="15"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="49"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="1:9" ht="16">
       <c r="A33" s="21" t="s">
@@ -1959,7 +1962,7 @@
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="48">
+      <c r="I33" s="57">
         <v>12</v>
       </c>
     </row>
@@ -1982,7 +1985,7 @@
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="49"/>
+      <c r="I34" s="58"/>
     </row>
     <row r="35" spans="1:9" ht="16">
       <c r="A35" s="21" t="s">
@@ -2001,7 +2004,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="11"/>
-      <c r="I35" s="48">
+      <c r="I35" s="57">
         <v>10</v>
       </c>
     </row>
@@ -2022,7 +2025,7 @@
         <v>4</v>
       </c>
       <c r="H36" s="16"/>
-      <c r="I36" s="49"/>
+      <c r="I36" s="58"/>
     </row>
     <row r="37" spans="1:9" ht="16">
       <c r="A37" s="21" t="s">
@@ -2035,7 +2038,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="48">
+      <c r="I37" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2050,7 +2053,7 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="49"/>
+      <c r="I38" s="58"/>
     </row>
     <row r="39" spans="1:9" ht="16">
       <c r="A39" s="21" t="s">
@@ -2069,7 +2072,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="19"/>
-      <c r="I39" s="48">
+      <c r="I39" s="57">
         <v>12</v>
       </c>
     </row>
@@ -2090,7 +2093,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="15"/>
       <c r="H40" s="14"/>
-      <c r="I40" s="49"/>
+      <c r="I40" s="58"/>
     </row>
     <row r="41" spans="1:9" ht="16">
       <c r="A41" s="21" t="s">
@@ -2109,7 +2112,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
-      <c r="I41" s="48">
+      <c r="I41" s="57">
         <v>17</v>
       </c>
     </row>
@@ -2130,7 +2133,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="15"/>
       <c r="H42" s="14"/>
-      <c r="I42" s="49"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="1:9" ht="16">
       <c r="A43" s="21" t="s">
@@ -2143,7 +2146,7 @@
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="20"/>
-      <c r="I43" s="48">
+      <c r="I43" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2158,7 +2161,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="15"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="49"/>
+      <c r="I44" s="58"/>
     </row>
     <row r="45" spans="1:9" ht="16">
       <c r="A45" s="29" t="s">
@@ -2190,13 +2193,13 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16">
-      <c r="A46" s="59" t="s">
+      <c r="A46" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2277,7 +2280,7 @@
       <c r="H49" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I49" s="48">
+      <c r="I49" s="57">
         <v>17</v>
       </c>
     </row>
@@ -2300,7 +2303,7 @@
       <c r="H50" s="16">
         <v>5</v>
       </c>
-      <c r="I50" s="49"/>
+      <c r="I50" s="58"/>
     </row>
     <row r="51" spans="1:9" ht="16">
       <c r="A51" s="21" t="s">
@@ -2313,7 +2316,7 @@
       <c r="F51" s="19"/>
       <c r="G51" s="18"/>
       <c r="H51" s="20"/>
-      <c r="I51" s="48">
+      <c r="I51" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2328,7 +2331,7 @@
       <c r="F52" s="14"/>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="49"/>
+      <c r="I52" s="58"/>
     </row>
     <row r="53" spans="1:9" ht="16">
       <c r="A53" s="21" t="s">
@@ -2351,7 +2354,7 @@
       <c r="H53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="48">
+      <c r="I53" s="57">
         <v>23.5</v>
       </c>
     </row>
@@ -2376,7 +2379,7 @@
       <c r="H54" s="16">
         <v>5</v>
       </c>
-      <c r="I54" s="49"/>
+      <c r="I54" s="58"/>
     </row>
     <row r="55" spans="1:9" ht="16">
       <c r="A55" s="21" t="s">
@@ -2399,7 +2402,7 @@
       <c r="H55" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="48">
+      <c r="I55" s="57">
         <v>19</v>
       </c>
     </row>
@@ -2424,7 +2427,7 @@
       <c r="H56" s="16">
         <v>3</v>
       </c>
-      <c r="I56" s="49"/>
+      <c r="I56" s="58"/>
     </row>
     <row r="57" spans="1:9" ht="16">
       <c r="A57" s="21" t="s">
@@ -2441,7 +2444,7 @@
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="H57" s="20"/>
-      <c r="I57" s="48">
+      <c r="I57" s="57">
         <v>9</v>
       </c>
     </row>
@@ -2460,7 +2463,7 @@
       <c r="F58" s="14"/>
       <c r="G58" s="15"/>
       <c r="H58" s="16"/>
-      <c r="I58" s="49"/>
+      <c r="I58" s="58"/>
     </row>
     <row r="59" spans="1:9" ht="16">
       <c r="A59" s="21" t="s">
@@ -2483,7 +2486,7 @@
       <c r="H59" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I59" s="48">
+      <c r="I59" s="57">
         <v>24.5</v>
       </c>
     </row>
@@ -2508,20 +2511,20 @@
       <c r="H60" s="14">
         <v>4</v>
       </c>
-      <c r="I60" s="49"/>
+      <c r="I60" s="58"/>
     </row>
     <row r="61" spans="1:9" ht="16">
       <c r="A61" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="62"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="64"/>
+      <c r="I61" s="65"/>
     </row>
     <row r="62" spans="1:9" ht="16">
       <c r="A62" s="21" t="s">
@@ -2534,7 +2537,7 @@
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
       <c r="H62" s="20"/>
-      <c r="I62" s="48">
+      <c r="I62" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2549,7 +2552,7 @@
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
       <c r="H63" s="16"/>
-      <c r="I63" s="49"/>
+      <c r="I63" s="58"/>
     </row>
     <row r="64" spans="1:9" ht="16">
       <c r="A64" s="21" t="s">
@@ -2566,7 +2569,7 @@
         <v>15</v>
       </c>
       <c r="H64" s="11"/>
-      <c r="I64" s="48">
+      <c r="I64" s="57">
         <v>7</v>
       </c>
     </row>
@@ -2585,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="H65" s="16"/>
-      <c r="I65" s="49"/>
+      <c r="I65" s="58"/>
     </row>
     <row r="66" spans="1:9" ht="16">
       <c r="A66" s="21" t="s">
@@ -2598,7 +2601,7 @@
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="25"/>
-      <c r="I66" s="48">
+      <c r="I66" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2613,7 +2616,7 @@
       <c r="F67" s="14"/>
       <c r="G67" s="15"/>
       <c r="H67" s="26"/>
-      <c r="I67" s="49"/>
+      <c r="I67" s="58"/>
     </row>
     <row r="68" spans="1:9" ht="16">
       <c r="A68" s="21" t="s">
@@ -2630,7 +2633,7 @@
       <c r="F68" s="27"/>
       <c r="G68" s="10"/>
       <c r="H68" s="11"/>
-      <c r="I68" s="48">
+      <c r="I68" s="57">
         <v>8</v>
       </c>
     </row>
@@ -2649,7 +2652,7 @@
       <c r="F69" s="14"/>
       <c r="G69" s="15"/>
       <c r="H69" s="16"/>
-      <c r="I69" s="49"/>
+      <c r="I69" s="58"/>
     </row>
     <row r="70" spans="1:9" ht="16">
       <c r="A70" s="21" t="s">
@@ -2672,7 +2675,7 @@
         <v>13</v>
       </c>
       <c r="H70" s="10"/>
-      <c r="I70" s="48">
+      <c r="I70" s="57">
         <v>19.5</v>
       </c>
     </row>
@@ -2697,7 +2700,7 @@
         <v>3</v>
       </c>
       <c r="H71" s="14"/>
-      <c r="I71" s="49"/>
+      <c r="I71" s="58"/>
     </row>
     <row r="72" spans="1:9" ht="16">
       <c r="A72" s="21" t="s">
@@ -2718,7 +2721,7 @@
         <v>14</v>
       </c>
       <c r="H72" s="11"/>
-      <c r="I72" s="48">
+      <c r="I72" s="57">
         <v>17</v>
       </c>
     </row>
@@ -2741,22 +2744,22 @@
         <v>5</v>
       </c>
       <c r="H73" s="16"/>
-      <c r="I73" s="49"/>
+      <c r="I73" s="58"/>
     </row>
     <row r="74" spans="1:9" ht="16">
       <c r="A74" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B74" s="56" t="s">
+      <c r="B74" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="57"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57"/>
-      <c r="H74" s="58"/>
-      <c r="I74" s="48">
+      <c r="C74" s="60"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="60"/>
+      <c r="F74" s="60"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="61"/>
+      <c r="I74" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2771,7 +2774,7 @@
       <c r="F75" s="14"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15"/>
-      <c r="I75" s="49"/>
+      <c r="I75" s="58"/>
     </row>
     <row r="76" spans="1:9" ht="16">
       <c r="A76" s="21" t="s">
@@ -2784,7 +2787,7 @@
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
       <c r="H76" s="11"/>
-      <c r="I76" s="48">
+      <c r="I76" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2799,7 +2802,7 @@
       <c r="F77" s="14"/>
       <c r="G77" s="15"/>
       <c r="H77" s="16"/>
-      <c r="I77" s="49"/>
+      <c r="I77" s="58"/>
     </row>
     <row r="78" spans="1:9" ht="16">
       <c r="A78" s="21" t="s">
@@ -2812,7 +2815,7 @@
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
       <c r="H78" s="20"/>
-      <c r="I78" s="48">
+      <c r="I78" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2827,7 +2830,7 @@
       <c r="F79" s="14"/>
       <c r="G79" s="15"/>
       <c r="H79" s="16"/>
-      <c r="I79" s="49"/>
+      <c r="I79" s="58"/>
     </row>
     <row r="80" spans="1:9" ht="16">
       <c r="A80" s="21" t="s">
@@ -2846,7 +2849,7 @@
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="11"/>
-      <c r="I80" s="48">
+      <c r="I80" s="57">
         <v>14.5</v>
       </c>
     </row>
@@ -2867,7 +2870,7 @@
       <c r="F81" s="14"/>
       <c r="G81" s="15"/>
       <c r="H81" s="16"/>
-      <c r="I81" s="49"/>
+      <c r="I81" s="58"/>
     </row>
     <row r="82" spans="1:9" ht="16">
       <c r="A82" s="21" t="s">
@@ -2880,7 +2883,7 @@
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
-      <c r="I82" s="48">
+      <c r="I82" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2895,7 +2898,7 @@
       <c r="F83" s="14"/>
       <c r="G83" s="15"/>
       <c r="H83" s="15"/>
-      <c r="I83" s="49"/>
+      <c r="I83" s="58"/>
     </row>
     <row r="84" spans="1:9" ht="16">
       <c r="A84" s="21" t="s">
@@ -2908,7 +2911,7 @@
       <c r="F84" s="19"/>
       <c r="G84" s="19"/>
       <c r="H84" s="19"/>
-      <c r="I84" s="48">
+      <c r="I84" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2923,7 +2926,7 @@
       <c r="F85" s="14"/>
       <c r="G85" s="15"/>
       <c r="H85" s="14"/>
-      <c r="I85" s="49"/>
+      <c r="I85" s="58"/>
     </row>
     <row r="86" spans="1:9" ht="16">
       <c r="A86" s="21" t="s">
@@ -2946,7 +2949,7 @@
       <c r="H86" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I86" s="48">
+      <c r="I86" s="57">
         <v>21.5</v>
       </c>
     </row>
@@ -2971,7 +2974,7 @@
       <c r="H87" s="14">
         <v>6.5</v>
       </c>
-      <c r="I87" s="49"/>
+      <c r="I87" s="58"/>
     </row>
     <row r="88" spans="1:9" ht="16">
       <c r="A88" s="21" t="s">
@@ -2984,7 +2987,7 @@
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
       <c r="H88" s="20"/>
-      <c r="I88" s="48">
+      <c r="I88" s="57">
         <v>0</v>
       </c>
     </row>
@@ -2999,7 +3002,7 @@
       <c r="F89" s="14"/>
       <c r="G89" s="15"/>
       <c r="H89" s="16"/>
-      <c r="I89" s="49"/>
+      <c r="I89" s="58"/>
     </row>
     <row r="90" spans="1:9" ht="17" thickBot="1">
       <c r="A90" s="29" t="s">
@@ -3031,149 +3034,149 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" thickTop="1">
-      <c r="A91" s="63" t="s">
+      <c r="A91" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B91" s="64"/>
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
-      <c r="F91" s="64"/>
-      <c r="G91" s="64"/>
-      <c r="H91" s="64"/>
-      <c r="I91" s="65"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
+      <c r="E91" s="49"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="49"/>
+      <c r="I91" s="50"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="66"/>
-      <c r="B92" s="67"/>
-      <c r="C92" s="67"/>
-      <c r="D92" s="67"/>
-      <c r="E92" s="67"/>
-      <c r="F92" s="67"/>
-      <c r="G92" s="67"/>
-      <c r="H92" s="67"/>
-      <c r="I92" s="68"/>
+      <c r="A92" s="51"/>
+      <c r="B92" s="52"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="52"/>
+      <c r="E92" s="52"/>
+      <c r="F92" s="52"/>
+      <c r="G92" s="52"/>
+      <c r="H92" s="52"/>
+      <c r="I92" s="53"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="66"/>
-      <c r="B93" s="67"/>
-      <c r="C93" s="67"/>
-      <c r="D93" s="67"/>
-      <c r="E93" s="67"/>
-      <c r="F93" s="67"/>
-      <c r="G93" s="67"/>
-      <c r="H93" s="67"/>
-      <c r="I93" s="68"/>
+      <c r="A93" s="51"/>
+      <c r="B93" s="52"/>
+      <c r="C93" s="52"/>
+      <c r="D93" s="52"/>
+      <c r="E93" s="52"/>
+      <c r="F93" s="52"/>
+      <c r="G93" s="52"/>
+      <c r="H93" s="52"/>
+      <c r="I93" s="53"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="66"/>
-      <c r="B94" s="67"/>
-      <c r="C94" s="67"/>
-      <c r="D94" s="67"/>
-      <c r="E94" s="67"/>
-      <c r="F94" s="67"/>
-      <c r="G94" s="67"/>
-      <c r="H94" s="67"/>
-      <c r="I94" s="68"/>
+      <c r="A94" s="51"/>
+      <c r="B94" s="52"/>
+      <c r="C94" s="52"/>
+      <c r="D94" s="52"/>
+      <c r="E94" s="52"/>
+      <c r="F94" s="52"/>
+      <c r="G94" s="52"/>
+      <c r="H94" s="52"/>
+      <c r="I94" s="53"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="66"/>
-      <c r="B95" s="67"/>
-      <c r="C95" s="67"/>
-      <c r="D95" s="67"/>
-      <c r="E95" s="67"/>
-      <c r="F95" s="67"/>
-      <c r="G95" s="67"/>
-      <c r="H95" s="67"/>
-      <c r="I95" s="68"/>
+      <c r="A95" s="51"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="52"/>
+      <c r="E95" s="52"/>
+      <c r="F95" s="52"/>
+      <c r="G95" s="52"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="53"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="66"/>
-      <c r="B96" s="67"/>
-      <c r="C96" s="67"/>
-      <c r="D96" s="67"/>
-      <c r="E96" s="67"/>
-      <c r="F96" s="67"/>
-      <c r="G96" s="67"/>
-      <c r="H96" s="67"/>
-      <c r="I96" s="68"/>
+      <c r="A96" s="51"/>
+      <c r="B96" s="52"/>
+      <c r="C96" s="52"/>
+      <c r="D96" s="52"/>
+      <c r="E96" s="52"/>
+      <c r="F96" s="52"/>
+      <c r="G96" s="52"/>
+      <c r="H96" s="52"/>
+      <c r="I96" s="53"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="66"/>
-      <c r="B97" s="67"/>
-      <c r="C97" s="67"/>
-      <c r="D97" s="67"/>
-      <c r="E97" s="67"/>
-      <c r="F97" s="67"/>
-      <c r="G97" s="67"/>
-      <c r="H97" s="67"/>
-      <c r="I97" s="68"/>
+      <c r="A97" s="51"/>
+      <c r="B97" s="52"/>
+      <c r="C97" s="52"/>
+      <c r="D97" s="52"/>
+      <c r="E97" s="52"/>
+      <c r="F97" s="52"/>
+      <c r="G97" s="52"/>
+      <c r="H97" s="52"/>
+      <c r="I97" s="53"/>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="66"/>
-      <c r="B98" s="67"/>
-      <c r="C98" s="67"/>
-      <c r="D98" s="67"/>
-      <c r="E98" s="67"/>
-      <c r="F98" s="67"/>
-      <c r="G98" s="67"/>
-      <c r="H98" s="67"/>
-      <c r="I98" s="68"/>
+      <c r="A98" s="51"/>
+      <c r="B98" s="52"/>
+      <c r="C98" s="52"/>
+      <c r="D98" s="52"/>
+      <c r="E98" s="52"/>
+      <c r="F98" s="52"/>
+      <c r="G98" s="52"/>
+      <c r="H98" s="52"/>
+      <c r="I98" s="53"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="66"/>
-      <c r="B99" s="67"/>
-      <c r="C99" s="67"/>
-      <c r="D99" s="67"/>
-      <c r="E99" s="67"/>
-      <c r="F99" s="67"/>
-      <c r="G99" s="67"/>
-      <c r="H99" s="67"/>
-      <c r="I99" s="68"/>
+      <c r="A99" s="51"/>
+      <c r="B99" s="52"/>
+      <c r="C99" s="52"/>
+      <c r="D99" s="52"/>
+      <c r="E99" s="52"/>
+      <c r="F99" s="52"/>
+      <c r="G99" s="52"/>
+      <c r="H99" s="52"/>
+      <c r="I99" s="53"/>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="66"/>
-      <c r="B100" s="67"/>
-      <c r="C100" s="67"/>
-      <c r="D100" s="67"/>
-      <c r="E100" s="67"/>
-      <c r="F100" s="67"/>
-      <c r="G100" s="67"/>
-      <c r="H100" s="67"/>
-      <c r="I100" s="68"/>
+      <c r="A100" s="51"/>
+      <c r="B100" s="52"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="52"/>
+      <c r="G100" s="52"/>
+      <c r="H100" s="52"/>
+      <c r="I100" s="53"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="66"/>
-      <c r="B101" s="67"/>
-      <c r="C101" s="67"/>
-      <c r="D101" s="67"/>
-      <c r="E101" s="67"/>
-      <c r="F101" s="67"/>
-      <c r="G101" s="67"/>
-      <c r="H101" s="67"/>
-      <c r="I101" s="68"/>
+      <c r="A101" s="51"/>
+      <c r="B101" s="52"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="52"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="52"/>
+      <c r="G101" s="52"/>
+      <c r="H101" s="52"/>
+      <c r="I101" s="53"/>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="66"/>
-      <c r="B102" s="67"/>
-      <c r="C102" s="67"/>
-      <c r="D102" s="67"/>
-      <c r="E102" s="67"/>
-      <c r="F102" s="67"/>
-      <c r="G102" s="67"/>
-      <c r="H102" s="67"/>
-      <c r="I102" s="68"/>
+      <c r="A102" s="51"/>
+      <c r="B102" s="52"/>
+      <c r="C102" s="52"/>
+      <c r="D102" s="52"/>
+      <c r="E102" s="52"/>
+      <c r="F102" s="52"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="52"/>
+      <c r="I102" s="53"/>
     </row>
     <row r="103" spans="1:9" ht="15" thickBot="1">
-      <c r="A103" s="69"/>
-      <c r="B103" s="70"/>
-      <c r="C103" s="70"/>
-      <c r="D103" s="70"/>
-      <c r="E103" s="70"/>
-      <c r="F103" s="70"/>
-      <c r="G103" s="70"/>
-      <c r="H103" s="70"/>
-      <c r="I103" s="71"/>
+      <c r="A103" s="54"/>
+      <c r="B103" s="55"/>
+      <c r="C103" s="55"/>
+      <c r="D103" s="55"/>
+      <c r="E103" s="55"/>
+      <c r="F103" s="55"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="56"/>
     </row>
     <row r="104" spans="1:9" ht="15" thickTop="1">
       <c r="A104" s="1"/>
@@ -3188,14 +3191,29 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A91:I103"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I80:I81"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I84:I85"/>
-    <mergeCell ref="I86:I87"/>
-    <mergeCell ref="I88:I89"/>
-    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="I33:I34"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="I49:I50"/>
     <mergeCell ref="I78:I79"/>
@@ -3212,29 +3230,14 @@
     <mergeCell ref="I74:I75"/>
     <mergeCell ref="I76:I77"/>
     <mergeCell ref="I51:I52"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A91:I103"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I80:I81"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="B74:H74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>